<commit_message>
Ajout du journal de bord dans le ficher journal de travail
</commit_message>
<xml_diff>
--- a/doc/journal de travail/journal de travail-Meline.Juillet.xlsx
+++ b/doc/journal de travail/journal de travail-Meline.Juillet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
+    <sheet name="Journal de board" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -135,13 +136,28 @@
   </si>
   <si>
     <t>Creation des Issues et des sprint.</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem avec git. Un merge as du etre fait car il y avais une différence entre git et github. </t>
+  </si>
+  <si>
+    <t>Aide de M.Favre.</t>
+  </si>
+  <si>
+    <t>Evénement</t>
+  </si>
+  <si>
+    <t>Initioation à la planification en mode agile de la part du mandant. Mise en place des date de rendu des sprint (chaque fin de semaine).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,8 +180,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +199,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -303,20 +333,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -626,15 +669,15 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="17"/>
       <c r="K1" s="10" t="s">
         <v>22</v>
@@ -653,22 +696,22 @@
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="11">
         <v>3</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
     </row>
     <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -683,16 +726,16 @@
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="11">
         <v>3</v>
       </c>
@@ -710,14 +753,14 @@
       <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
       <c r="K4" s="11">
         <v>3</v>
       </c>
@@ -735,14 +778,14 @@
       <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="12">
         <v>3</v>
       </c>
@@ -760,16 +803,16 @@
       <c r="D6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="12">
         <v>3</v>
       </c>
@@ -787,16 +830,16 @@
       <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15" t="s">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="12">
         <v>3</v>
       </c>
@@ -814,14 +857,14 @@
       <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="12">
         <v>4</v>
       </c>
@@ -839,14 +882,14 @@
       <c r="D9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="12">
         <v>4</v>
       </c>
@@ -864,14 +907,14 @@
       <c r="D10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="12">
         <v>4</v>
       </c>
@@ -889,16 +932,16 @@
       <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="12">
         <v>4</v>
       </c>
@@ -916,16 +959,16 @@
       <c r="D12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="12">
         <v>4</v>
       </c>
@@ -943,14 +986,14 @@
       <c r="D13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="12">
         <v>5</v>
       </c>
@@ -968,42 +1011,60 @@
       <c r="D14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="12"/>
+    <row r="15" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>43901</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="9">
+        <v>43901</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1011,12 +1072,12 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1024,12 +1085,12 @@
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1037,12 +1098,12 @@
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1050,12 +1111,12 @@
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1063,12 +1124,12 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1076,12 +1137,12 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1089,12 +1150,12 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1102,12 +1163,12 @@
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1115,12 +1176,12 @@
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1128,12 +1189,12 @@
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
       <c r="K26" s="12"/>
     </row>
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -1141,38 +1202,33 @@
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
       <c r="K27" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G1:J1"/>
@@ -1189,23 +1245,28 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G14:J14"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D16">
@@ -1218,4 +1279,120 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23">
+        <v>43901</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modification de la grille
</commit_message>
<xml_diff>
--- a/doc/journal de travail/journal de travail-Meline.Juillet.xlsx
+++ b/doc/journal de travail/journal de travail-Meline.Juillet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Clion\MA-20\Bataille-Navale.Meline.Juillet\doc\journal de travail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Clion_Exercises\Bataille navale\Bataille-Navale\doc\journal de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73467834-633E-46E2-85CA-A2E23DB0CDD2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -151,12 +152,18 @@
   </si>
   <si>
     <t>Initioation à la planification en mode agile de la part du mandant. Mise en place des date de rendu des sprint (chaque fin de semaine).</t>
+  </si>
+  <si>
+    <t>Finition du point de vue graphique du programme et régralge des différent problem de tableau.</t>
+  </si>
+  <si>
+    <t>Création du journal de board et lecture du support de cours.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -333,33 +340,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,23 +647,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.75" customWidth="1"/>
-    <col min="3" max="3" width="19.75" customWidth="1"/>
-    <col min="4" max="4" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" customWidth="1"/>
+    <col min="3" max="3" width="19.69921875" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
     <col min="11" max="11" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,21 +676,21 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="17"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
       <c r="K1" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43887</v>
       </c>
@@ -696,24 +703,24 @@
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
       <c r="K2" s="11">
         <v>3</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-    </row>
-    <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43887</v>
       </c>
@@ -726,21 +733,21 @@
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43887</v>
       </c>
@@ -753,19 +760,19 @@
       <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>43888</v>
       </c>
@@ -778,19 +785,19 @@
       <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
       <c r="K5" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>43888</v>
       </c>
@@ -803,21 +810,21 @@
       <c r="D6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
       <c r="K6" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>43889</v>
       </c>
@@ -830,21 +837,21 @@
       <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
       <c r="K7" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>43894</v>
       </c>
@@ -857,19 +864,19 @@
       <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
       <c r="K8" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>43894</v>
       </c>
@@ -882,19 +889,19 @@
       <c r="D9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>43894</v>
       </c>
@@ -907,19 +914,19 @@
       <c r="D10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>43895</v>
       </c>
@@ -932,21 +939,21 @@
       <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="17"/>
+      <c r="G11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
       <c r="K11" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>43896</v>
       </c>
@@ -959,21 +966,21 @@
       <c r="D12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
       <c r="K12" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>43901</v>
       </c>
@@ -986,19 +993,19 @@
       <c r="D13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
       <c r="K13" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>43901</v>
       </c>
@@ -1011,19 +1018,19 @@
       <c r="D14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>43901</v>
       </c>
@@ -1036,199 +1043,220 @@
       <c r="D15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14" t="s">
+      <c r="F15" s="17"/>
+      <c r="G15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
       <c r="K15" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>43901</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="C16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+    <row r="17" spans="1:11" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>43901</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
       <c r="K27" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G1:J1"/>
@@ -1245,34 +1273,29 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G9:J9"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ICT-114,ICT-431,ICT-101,IEL3,MA-20,MA-10,MA-9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Théorie, Exercices pratique, Exercices personnel, Correction, Absence, travail pratique,Explication"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1282,103 +1305,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
         <v>43901</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>